<commit_message>
Auto-committed on 2021/12/08 週三
Former-commit-id: ae254907f99279d6ae1739a3931c2afb9219b16f
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L2-業務作業/CustDataCtrl.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L2-業務作業/CustDataCtrl.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L2-業務作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\SKL\DB\GenTables\L2-業務作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20916" windowHeight="8472"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="15710" windowHeight="5850"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -792,21 +792,21 @@
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="21.453125" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="21.44140625" style="4"/>
+    <col min="7" max="7" width="27.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="21.453125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>21</v>
       </c>
@@ -821,7 +821,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="19"/>
       <c r="B2" s="20"/>
       <c r="C2" s="12" t="s">
@@ -834,7 +834,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>23</v>
       </c>
@@ -847,7 +847,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="19" t="s">
         <v>24</v>
       </c>
@@ -862,7 +862,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
         <v>25</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="19" t="s">
         <v>26</v>
       </c>
@@ -884,7 +884,7 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="19" t="s">
         <v>27</v>
       </c>
@@ -895,7 +895,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="12" t="s">
         <v>28</v>
       </c>
@@ -918,7 +918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="18">
         <v>2</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="1:7" ht="81" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.4">
       <c r="A11" s="18">
         <v>3</v>
       </c>
@@ -977,7 +977,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="18">
         <v>4</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="18">
         <v>5</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" s="18">
         <v>6</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="18">
         <v>7</v>
       </c>
@@ -1049,7 +1049,7 @@
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" s="18">
         <v>8</v>
       </c>
@@ -1068,7 +1068,7 @@
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -1077,7 +1077,7 @@
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -1086,7 +1086,7 @@
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -1095,7 +1095,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -1104,7 +1104,7 @@
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -1113,7 +1113,7 @@
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1122,7 +1122,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -1131,7 +1131,7 @@
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -1140,7 +1140,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -1149,7 +1149,7 @@
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -1158,7 +1158,7 @@
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -1167,7 +1167,7 @@
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -1176,7 +1176,7 @@
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -1185,7 +1185,7 @@
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -1194,7 +1194,7 @@
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -1203,7 +1203,7 @@
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1212,7 +1212,7 @@
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -1221,7 +1221,7 @@
       <c r="F33" s="18"/>
       <c r="G33" s="18"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -1230,7 +1230,7 @@
       <c r="F34" s="18"/>
       <c r="G34" s="18"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -1239,7 +1239,7 @@
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -1248,7 +1248,7 @@
       <c r="F36" s="18"/>
       <c r="G36" s="18"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -1257,7 +1257,7 @@
       <c r="F37" s="18"/>
       <c r="G37" s="18"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -1266,7 +1266,7 @@
       <c r="F38" s="18"/>
       <c r="G38" s="18"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="18"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -1275,7 +1275,7 @@
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -1284,7 +1284,7 @@
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="18"/>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -1293,7 +1293,7 @@
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -1302,7 +1302,7 @@
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -1311,7 +1311,7 @@
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
@@ -1320,7 +1320,7 @@
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
@@ -1329,7 +1329,7 @@
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -1338,7 +1338,7 @@
       <c r="F46" s="18"/>
       <c r="G46" s="18"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -1347,7 +1347,7 @@
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48" s="18"/>
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
@@ -1356,7 +1356,7 @@
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
@@ -1365,7 +1365,7 @@
       <c r="F49" s="18"/>
       <c r="G49" s="18"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -1374,7 +1374,7 @@
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -1383,7 +1383,7 @@
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52" s="18"/>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
@@ -1392,7 +1392,7 @@
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53" s="18"/>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -1401,7 +1401,7 @@
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -1410,7 +1410,7 @@
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55" s="18"/>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -1419,7 +1419,7 @@
       <c r="F55" s="18"/>
       <c r="G55" s="18"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56" s="18"/>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
@@ -1428,7 +1428,7 @@
       <c r="F56" s="18"/>
       <c r="G56" s="18"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57" s="18"/>
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
@@ -1437,7 +1437,7 @@
       <c r="F57" s="18"/>
       <c r="G57" s="18"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58" s="18"/>
       <c r="B58" s="18"/>
       <c r="C58" s="18"/>
@@ -1446,7 +1446,7 @@
       <c r="F58" s="18"/>
       <c r="G58" s="18"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59" s="18"/>
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
@@ -1455,7 +1455,7 @@
       <c r="F59" s="18"/>
       <c r="G59" s="18"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60" s="18"/>
       <c r="B60" s="18"/>
       <c r="C60" s="18"/>
@@ -1464,7 +1464,7 @@
       <c r="F60" s="18"/>
       <c r="G60" s="18"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61" s="18"/>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -1473,7 +1473,7 @@
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A62" s="18"/>
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
@@ -1482,7 +1482,7 @@
       <c r="F62" s="18"/>
       <c r="G62" s="18"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A63" s="18"/>
       <c r="B63" s="18"/>
       <c r="C63" s="18"/>
@@ -1491,7 +1491,7 @@
       <c r="F63" s="18"/>
       <c r="G63" s="18"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A64" s="18"/>
       <c r="B64" s="18"/>
       <c r="C64" s="18"/>
@@ -1500,7 +1500,7 @@
       <c r="F64" s="18"/>
       <c r="G64" s="18"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A65" s="18"/>
       <c r="B65" s="18"/>
       <c r="C65" s="18"/>
@@ -1509,7 +1509,7 @@
       <c r="F65" s="18"/>
       <c r="G65" s="18"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66" s="18"/>
       <c r="B66" s="18"/>
       <c r="C66" s="18"/>
@@ -1518,7 +1518,7 @@
       <c r="F66" s="18"/>
       <c r="G66" s="18"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67" s="18"/>
       <c r="B67" s="18"/>
       <c r="C67" s="18"/>
@@ -1527,7 +1527,7 @@
       <c r="F67" s="18"/>
       <c r="G67" s="18"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68" s="18"/>
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
@@ -1536,7 +1536,7 @@
       <c r="F68" s="18"/>
       <c r="G68" s="18"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69" s="18"/>
       <c r="B69" s="18"/>
       <c r="C69" s="18"/>
@@ -1545,7 +1545,7 @@
       <c r="F69" s="18"/>
       <c r="G69" s="18"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70" s="18"/>
       <c r="B70" s="18"/>
       <c r="C70" s="18"/>
@@ -1554,7 +1554,7 @@
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A71" s="18"/>
       <c r="B71" s="18"/>
       <c r="C71" s="18"/>
@@ -1563,7 +1563,7 @@
       <c r="F71" s="18"/>
       <c r="G71" s="18"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72" s="18"/>
       <c r="B72" s="18"/>
       <c r="C72" s="18"/>
@@ -1572,7 +1572,7 @@
       <c r="F72" s="18"/>
       <c r="G72" s="18"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A73" s="18"/>
       <c r="B73" s="18"/>
       <c r="C73" s="18"/>
@@ -1581,7 +1581,7 @@
       <c r="F73" s="18"/>
       <c r="G73" s="18"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A74" s="18"/>
       <c r="B74" s="18"/>
       <c r="C74" s="18"/>
@@ -1612,18 +1612,18 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.08984375" style="2" customWidth="1"/>
     <col min="3" max="3" width="17" style="2" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>

</xml_diff>